<commit_message>
Implemented Machine Learning ARIMA Predictions
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,7 +455,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>CO (ppm)</t>
+          <t>Feels Like</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Pressure</t>
         </is>
       </c>
     </row>
@@ -464,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45281</v>
+        <v>45283</v>
       </c>
       <c r="C2" t="n">
         <v>20.62178083193154</v>
@@ -474,6 +479,9 @@
       </c>
       <c r="E2" t="n">
         <v>1.424202471887338</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.626998490796339</v>
       </c>
     </row>
     <row r="3">
@@ -481,7 +489,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45281.04166666666</v>
+        <v>45283.04166666666</v>
       </c>
       <c r="C3" t="n">
         <v>24.65500014486941</v>
@@ -491,6 +499,9 @@
       </c>
       <c r="E3" t="n">
         <v>0.184434736772664</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3.732457025590121</v>
       </c>
     </row>
     <row r="4">
@@ -498,7 +509,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45281.08333333334</v>
+        <v>45283.08333333334</v>
       </c>
       <c r="C4" t="n">
         <v>23.12395759267984</v>
@@ -508,6 +519,9 @@
       </c>
       <c r="E4" t="n">
         <v>3.047821669899484</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.248164495236074</v>
       </c>
     </row>
     <row r="5">
@@ -515,7 +529,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45281.125</v>
+        <v>45283.125</v>
       </c>
       <c r="C5" t="n">
         <v>22.19060938937925</v>
@@ -525,6 +539,9 @@
       </c>
       <c r="E5" t="n">
         <v>2.513395116144308</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4.24611705247089</v>
       </c>
     </row>
     <row r="6">
@@ -532,7 +549,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45281.16666666666</v>
+        <v>45283.16666666666</v>
       </c>
       <c r="C6" t="n">
         <v>19.09213048309705</v>
@@ -542,6 +559,9 @@
       </c>
       <c r="E6" t="n">
         <v>0.2573937562499468</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.288064461501717</v>
       </c>
     </row>
     <row r="7">
@@ -549,7 +569,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45281.20833333334</v>
+        <v>45283.20833333334</v>
       </c>
       <c r="C7" t="n">
         <v>19.09196164235342</v>
@@ -559,6 +579,9 @@
       </c>
       <c r="E7" t="n">
         <v>1.393232321183057</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2.841543016677358</v>
       </c>
     </row>
     <row r="8">
@@ -566,7 +589,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45281.25</v>
+        <v>45283.25</v>
       </c>
       <c r="C8" t="n">
         <v>18.4065852851774</v>
@@ -576,6 +599,9 @@
       </c>
       <c r="E8" t="n">
         <v>4.541329429833269</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.4683738391404624</v>
       </c>
     </row>
     <row r="9">
@@ -583,7 +609,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45281.29166666666</v>
+        <v>45283.29166666666</v>
       </c>
       <c r="C9" t="n">
         <v>24.06323302042455</v>
@@ -593,6 +619,9 @@
       </c>
       <c r="E9" t="n">
         <v>1.197809453334862</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.838579015297168</v>
       </c>
     </row>
     <row r="10">
@@ -600,7 +629,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45281.33333333334</v>
+        <v>45283.33333333334</v>
       </c>
       <c r="C10" t="n">
         <v>22.20780508220246</v>
@@ -610,6 +639,9 @@
       </c>
       <c r="E10" t="n">
         <v>0.7244743604561155</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.326011838408627</v>
       </c>
     </row>
     <row r="11">
@@ -617,7 +649,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45281.375</v>
+        <v>45283.375</v>
       </c>
       <c r="C11" t="n">
         <v>22.95650804457232</v>
@@ -627,6 +659,9 @@
       </c>
       <c r="E11" t="n">
         <v>2.447263801387815</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.219948216895418</v>
       </c>
     </row>
     <row r="12">
@@ -634,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>45281.41666666666</v>
+        <v>45283.41666666666</v>
       </c>
       <c r="C12" t="n">
         <v>18.14409146007062</v>
@@ -644,6 +679,9 @@
       </c>
       <c r="E12" t="n">
         <v>4.928252270553004</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4.865052773762228</v>
       </c>
     </row>
     <row r="13">
@@ -651,7 +689,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45281.45833333334</v>
+        <v>45283.45833333334</v>
       </c>
       <c r="C13" t="n">
         <v>24.78936896513396</v>
@@ -661,6 +699,9 @@
       </c>
       <c r="E13" t="n">
         <v>1.210276357557502</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.965488623333802</v>
       </c>
     </row>
     <row r="14">
@@ -668,7 +709,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45281.5</v>
+        <v>45283.5</v>
       </c>
       <c r="C14" t="n">
         <v>23.82709848560295</v>
@@ -678,6 +719,9 @@
       </c>
       <c r="E14" t="n">
         <v>3.360677737029393</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4.460232775885567</v>
       </c>
     </row>
     <row r="15">
@@ -685,7 +729,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45281.54166666666</v>
+        <v>45283.54166666666</v>
       </c>
       <c r="C15" t="n">
         <v>19.48637377474793</v>
@@ -695,6 +739,9 @@
       </c>
       <c r="E15" t="n">
         <v>3.808098076643588</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3.155693129986314</v>
       </c>
     </row>
     <row r="16">
@@ -702,7 +749,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45281.58333333334</v>
+        <v>45283.58333333334</v>
       </c>
       <c r="C16" t="n">
         <v>19.2727747704497</v>
@@ -712,6 +759,9 @@
       </c>
       <c r="E16" t="n">
         <v>1.188187719961998</v>
+      </c>
+      <c r="F16" t="n">
+        <v>3.974056517708242</v>
       </c>
     </row>
     <row r="17">
@@ -719,7 +769,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45281.625</v>
+        <v>45283.625</v>
       </c>
       <c r="C17" t="n">
         <v>19.28383156897404</v>
@@ -729,6 +779,9 @@
       </c>
       <c r="E17" t="n">
         <v>3.641081743059298</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2.51318546552596</v>
       </c>
     </row>
     <row r="18">
@@ -736,7 +789,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45281.66666666666</v>
+        <v>45283.66666666666</v>
       </c>
       <c r="C18" t="n">
         <v>20.12969570071676</v>
@@ -746,6 +799,9 @@
       </c>
       <c r="E18" t="n">
         <v>1.838915663596266</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2.884519423131795</v>
       </c>
     </row>
     <row r="19">
@@ -753,7 +809,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>45281.70833333334</v>
+        <v>45283.70833333334</v>
       </c>
       <c r="C19" t="n">
         <v>21.67329502142567</v>
@@ -763,6 +819,9 @@
       </c>
       <c r="E19" t="n">
         <v>3.161529152967897</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2.46258846909432</v>
       </c>
     </row>
     <row r="20">
@@ -770,7 +829,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>45281.75</v>
+        <v>45283.75</v>
       </c>
       <c r="C20" t="n">
         <v>21.02361513049481</v>
@@ -780,6 +839,9 @@
       </c>
       <c r="E20" t="n">
         <v>3.167648553804474</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.9762149389902225</v>
       </c>
     </row>
     <row r="21">
@@ -787,7 +849,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>45281.79166666666</v>
+        <v>45283.79166666666</v>
       </c>
       <c r="C21" t="n">
         <v>20.0386039813863</v>
@@ -797,6 +859,9 @@
       </c>
       <c r="E21" t="n">
         <v>2.678873420373793</v>
+      </c>
+      <c r="F21" t="n">
+        <v>3.612260576307527</v>
       </c>
     </row>
     <row r="22">
@@ -804,7 +869,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>45281.83333333334</v>
+        <v>45283.83333333334</v>
       </c>
       <c r="C22" t="n">
         <v>22.28297026305665</v>
@@ -814,6 +879,9 @@
       </c>
       <c r="E22" t="n">
         <v>0.4514488502720415</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1.403861812204279</v>
       </c>
     </row>
     <row r="23">
@@ -821,7 +889,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>45281.875</v>
+        <v>45283.875</v>
       </c>
       <c r="C23" t="n">
         <v>18.97645702456429</v>
@@ -831,6 +899,9 @@
       </c>
       <c r="E23" t="n">
         <v>4.17651247794619</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.1215798321572692</v>
       </c>
     </row>
     <row r="24">
@@ -838,7 +909,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>45281.91666666666</v>
+        <v>45283.91666666666</v>
       </c>
       <c r="C24" t="n">
         <v>20.04501253974653</v>
@@ -848,6 +919,9 @@
       </c>
       <c r="E24" t="n">
         <v>1.603900324858679</v>
+      </c>
+      <c r="F24" t="n">
+        <v>3.227361479535839</v>
       </c>
     </row>
     <row r="25">
@@ -855,7 +929,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>45281.95833333334</v>
+        <v>45283.95833333334</v>
       </c>
       <c r="C25" t="n">
         <v>20.56453290305584</v>
@@ -865,6 +939,9 @@
       </c>
       <c r="E25" t="n">
         <v>0.9325925519992712</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.8855533970352447</v>
       </c>
     </row>
     <row r="26">
@@ -872,7 +949,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>45282</v>
+        <v>45284</v>
       </c>
       <c r="C26" t="n">
         <v>21.19248988951925</v>
@@ -882,6 +959,9 @@
       </c>
       <c r="E26" t="n">
         <v>0.2038757077738196</v>
+      </c>
+      <c r="F26" t="n">
+        <v>4.702292921764571</v>
       </c>
     </row>
     <row r="27">
@@ -889,7 +969,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>45282.04166666666</v>
+        <v>45284.04166666666</v>
       </c>
       <c r="C27" t="n">
         <v>23.49623172975109</v>
@@ -899,6 +979,9 @@
       </c>
       <c r="E27" t="n">
         <v>2.954464715941209</v>
+      </c>
+      <c r="F27" t="n">
+        <v>4.769642885012937</v>
       </c>
     </row>
     <row r="28">
@@ -906,7 +989,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>45282.08333333334</v>
+        <v>45284.08333333334</v>
       </c>
       <c r="C28" t="n">
         <v>19.39771647510852</v>
@@ -916,6 +999,9 @@
       </c>
       <c r="E28" t="n">
         <v>3.387821809211412</v>
+      </c>
+      <c r="F28" t="n">
+        <v>4.574321951102243</v>
       </c>
     </row>
     <row r="29">
@@ -923,7 +1009,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>45282.125</v>
+        <v>45284.125</v>
       </c>
       <c r="C29" t="n">
         <v>21.59964106889528</v>
@@ -933,6 +1019,9 @@
       </c>
       <c r="E29" t="n">
         <v>0.08293914463928076</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1.850793501277222</v>
       </c>
     </row>
     <row r="30">
@@ -940,7 +1029,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>45282.16666666666</v>
+        <v>45284.16666666666</v>
       </c>
       <c r="C30" t="n">
         <v>22.1469019820343</v>
@@ -950,6 +1039,9 @@
       </c>
       <c r="E30" t="n">
         <v>2.560465291496405</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.07728308264433714</v>
       </c>
     </row>
     <row r="31">
@@ -957,7 +1049,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>45282.20833333334</v>
+        <v>45284.20833333334</v>
       </c>
       <c r="C31" t="n">
         <v>18.32515288903998</v>
@@ -967,6 +1059,9 @@
       </c>
       <c r="E31" t="n">
         <v>1.13247887598969</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4.641592812938627</v>
       </c>
     </row>
     <row r="32">
@@ -974,7 +1069,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>45282.25</v>
+        <v>45284.25</v>
       </c>
       <c r="C32" t="n">
         <v>22.25281396331007</v>
@@ -984,6 +1079,9 @@
       </c>
       <c r="E32" t="n">
         <v>3.225863952047249</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2.140920741586572</v>
       </c>
     </row>
     <row r="33">
@@ -991,7 +1089,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>45282.29166666666</v>
+        <v>45284.29166666666</v>
       </c>
       <c r="C33" t="n">
         <v>19.19366886581104</v>
@@ -1001,6 +1099,9 @@
       </c>
       <c r="E33" t="n">
         <v>0.8718321450249572</v>
+      </c>
+      <c r="F33" t="n">
+        <v>4.833274095218348</v>
       </c>
     </row>
     <row r="34">
@@ -1008,7 +1109,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45282.33333333334</v>
+        <v>45284.33333333334</v>
       </c>
       <c r="C34" t="n">
         <v>18.45536115089696</v>
@@ -1018,6 +1119,9 @@
       </c>
       <c r="E34" t="n">
         <v>3.45468869051233</v>
+      </c>
+      <c r="F34" t="n">
+        <v>4.818099885446264</v>
       </c>
     </row>
     <row r="35">
@@ -1025,7 +1129,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>45282.375</v>
+        <v>45284.375</v>
       </c>
       <c r="C35" t="n">
         <v>24.64219876077333</v>
@@ -1035,6 +1139,9 @@
       </c>
       <c r="E35" t="n">
         <v>1.933676731502687</v>
+      </c>
+      <c r="F35" t="n">
+        <v>4.265047277336801</v>
       </c>
     </row>
     <row r="36">
@@ -1042,7 +1149,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>45282.41666666666</v>
+        <v>45284.41666666666</v>
       </c>
       <c r="C36" t="n">
         <v>24.75942423152192</v>
@@ -1052,6 +1159,9 @@
       </c>
       <c r="E36" t="n">
         <v>4.683649943683672</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1.472244460347929</v>
       </c>
     </row>
     <row r="37">
@@ -1059,7 +1169,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>45282.45833333334</v>
+        <v>45284.45833333334</v>
       </c>
       <c r="C37" t="n">
         <v>23.65878143681523</v>
@@ -1069,6 +1179,9 @@
       </c>
       <c r="E37" t="n">
         <v>0.6876047207299663</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1.925488643009626</v>
       </c>
     </row>
     <row r="38">
@@ -1076,7 +1189,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>45282.5</v>
+        <v>45284.5</v>
       </c>
       <c r="C38" t="n">
         <v>20.1322963842136</v>
@@ -1086,6 +1199,9 @@
       </c>
       <c r="E38" t="n">
         <v>1.705331755251293</v>
+      </c>
+      <c r="F38" t="n">
+        <v>4.255683357584284</v>
       </c>
     </row>
     <row r="39">
@@ -1093,7 +1209,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>45282.54166666666</v>
+        <v>45284.54166666666</v>
       </c>
       <c r="C39" t="n">
         <v>18.68370479804469</v>
@@ -1103,6 +1219,9 @@
       </c>
       <c r="E39" t="n">
         <v>0.5673676062029454</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1.584610025781388</v>
       </c>
     </row>
     <row r="40">
@@ -1110,7 +1229,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>45282.58333333334</v>
+        <v>45284.58333333334</v>
       </c>
       <c r="C40" t="n">
         <v>22.7896311855851</v>
@@ -1120,6 +1239,9 @@
       </c>
       <c r="E40" t="n">
         <v>4.623468091392814</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.8474637334304624</v>
       </c>
     </row>
     <row r="41">
@@ -1127,7 +1249,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>45282.625</v>
+        <v>45284.625</v>
       </c>
       <c r="C41" t="n">
         <v>21.08106745617721</v>
@@ -1137,6 +1259,9 @@
       </c>
       <c r="E41" t="n">
         <v>4.386696766904905</v>
+      </c>
+      <c r="F41" t="n">
+        <v>2.784006312291751</v>
       </c>
     </row>
     <row r="42">
@@ -1144,7 +1269,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>45282.66666666666</v>
+        <v>45284.66666666666</v>
       </c>
       <c r="C42" t="n">
         <v>18.85426764391345</v>
@@ -1154,6 +1279,9 @@
       </c>
       <c r="E42" t="n">
         <v>1.289708138575778</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4.680773870803905</v>
       </c>
     </row>
     <row r="43">
@@ -1161,7 +1289,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>45282.70833333334</v>
+        <v>45284.70833333334</v>
       </c>
       <c r="C43" t="n">
         <v>21.46623837077889</v>
@@ -1171,6 +1299,9 @@
       </c>
       <c r="E43" t="n">
         <v>3.299920230170895</v>
+      </c>
+      <c r="F43" t="n">
+        <v>3.480148983374865</v>
       </c>
     </row>
     <row r="44">
@@ -1178,7 +1309,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>45282.75</v>
+        <v>45284.75</v>
       </c>
       <c r="C44" t="n">
         <v>18.24071964780653</v>
@@ -1188,6 +1319,9 @@
       </c>
       <c r="E44" t="n">
         <v>4.086111001006079</v>
+      </c>
+      <c r="F44" t="n">
+        <v>2.850305850446825</v>
       </c>
     </row>
     <row r="45">
@@ -1195,7 +1329,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>45282.79166666666</v>
+        <v>45284.79166666666</v>
       </c>
       <c r="C45" t="n">
         <v>24.36524281455148</v>
@@ -1205,6 +1339,9 @@
       </c>
       <c r="E45" t="n">
         <v>2.776004057997312</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.4858824688538427</v>
       </c>
     </row>
     <row r="46">
@@ -1212,7 +1349,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>45282.83333333334</v>
+        <v>45284.83333333334</v>
       </c>
       <c r="C46" t="n">
         <v>19.81145987120012</v>
@@ -1222,6 +1359,9 @@
       </c>
       <c r="E46" t="n">
         <v>2.648252891780032</v>
+      </c>
+      <c r="F46" t="n">
+        <v>3.075036133495849</v>
       </c>
     </row>
     <row r="47">
@@ -1229,7 +1369,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>45282.875</v>
+        <v>45284.875</v>
       </c>
       <c r="C47" t="n">
         <v>22.63765599047787</v>
@@ -1239,6 +1379,9 @@
       </c>
       <c r="E47" t="n">
         <v>1.209261454502258</v>
+      </c>
+      <c r="F47" t="n">
+        <v>4.950269250521316</v>
       </c>
     </row>
     <row r="48">
@@ -1246,7 +1389,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>45282.91666666666</v>
+        <v>45284.91666666666</v>
       </c>
       <c r="C48" t="n">
         <v>20.18197753262588</v>
@@ -1256,6 +1399,9 @@
       </c>
       <c r="E48" t="n">
         <v>0.4655138390294961</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.7004200761826201</v>
       </c>
     </row>
     <row r="49">
@@ -1263,7 +1409,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>45282.95833333334</v>
+        <v>45284.95833333334</v>
       </c>
       <c r="C49" t="n">
         <v>21.64047614824468</v>
@@ -1273,6 +1419,9 @@
       </c>
       <c r="E49" t="n">
         <v>4.486078789766633</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2.591648261818684</v>
       </c>
     </row>
     <row r="50">
@@ -1280,7 +1429,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>45283</v>
+        <v>45285</v>
       </c>
       <c r="C50" t="n">
         <v>21.82697195540296</v>
@@ -1290,6 +1439,9 @@
       </c>
       <c r="E50" t="n">
         <v>4.502090285816652</v>
+      </c>
+      <c r="F50" t="n">
+        <v>4.386865359639777</v>
       </c>
     </row>
     <row r="51">
@@ -1297,7 +1449,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>45283.04166666666</v>
+        <v>45285.04166666666</v>
       </c>
       <c r="C51" t="n">
         <v>19.29398118867869</v>
@@ -1307,6 +1459,9 @@
       </c>
       <c r="E51" t="n">
         <v>3.16550728636634</v>
+      </c>
+      <c r="F51" t="n">
+        <v>3.703843088771022</v>
       </c>
     </row>
     <row r="52">
@@ -1314,7 +1469,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>45283.08333333334</v>
+        <v>45285.08333333334</v>
       </c>
       <c r="C52" t="n">
         <v>24.78709239435191</v>
@@ -1324,6 +1479,9 @@
       </c>
       <c r="E52" t="n">
         <v>1.695148955243504</v>
+      </c>
+      <c r="F52" t="n">
+        <v>3.48507870497634</v>
       </c>
     </row>
     <row r="53">
@@ -1331,7 +1489,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>45283.125</v>
+        <v>45285.125</v>
       </c>
       <c r="C53" t="n">
         <v>23.4259297635278</v>
@@ -1341,6 +1499,9 @@
       </c>
       <c r="E53" t="n">
         <v>1.746047873063304</v>
+      </c>
+      <c r="F53" t="n">
+        <v>3.512420419935546</v>
       </c>
     </row>
     <row r="54">
@@ -1348,7 +1509,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>45283.16666666666</v>
+        <v>45285.16666666666</v>
       </c>
       <c r="C54" t="n">
         <v>24.57649259094933</v>
@@ -1358,6 +1519,9 @@
       </c>
       <c r="E54" t="n">
         <v>3.629778394351197</v>
+      </c>
+      <c r="F54" t="n">
+        <v>1.797455756098776</v>
       </c>
     </row>
     <row r="55">
@@ -1365,7 +1529,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="2" t="n">
-        <v>45283.20833333334</v>
+        <v>45285.20833333334</v>
       </c>
       <c r="C55" t="n">
         <v>24.26379145299354</v>
@@ -1375,6 +1539,9 @@
       </c>
       <c r="E55" t="n">
         <v>4.485551299762886</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1.467959221322467</v>
       </c>
     </row>
     <row r="56">
@@ -1382,7 +1549,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="2" t="n">
-        <v>45283.25</v>
+        <v>45285.25</v>
       </c>
       <c r="C56" t="n">
         <v>22.18529985167759</v>
@@ -1392,6 +1559,9 @@
       </c>
       <c r="E56" t="n">
         <v>4.435432121325587</v>
+      </c>
+      <c r="F56" t="n">
+        <v>4.046805777392568</v>
       </c>
     </row>
     <row r="57">
@@ -1399,7 +1569,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>45283.29166666666</v>
+        <v>45285.29166666666</v>
       </c>
       <c r="C57" t="n">
         <v>24.45311964516182</v>
@@ -1409,6 +1579,9 @@
       </c>
       <c r="E57" t="n">
         <v>3.899377729288119</v>
+      </c>
+      <c r="F57" t="n">
+        <v>4.050566973395904</v>
       </c>
     </row>
     <row r="58">
@@ -1416,7 +1589,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="2" t="n">
-        <v>45283.33333333334</v>
+        <v>45285.33333333334</v>
       </c>
       <c r="C58" t="n">
         <v>18.61944751436344</v>
@@ -1426,6 +1599,9 @@
       </c>
       <c r="E58" t="n">
         <v>3.210158230771439</v>
+      </c>
+      <c r="F58" t="n">
+        <v>4.335361592900519</v>
       </c>
     </row>
     <row r="59">
@@ -1433,7 +1609,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="2" t="n">
-        <v>45283.375</v>
+        <v>45285.375</v>
       </c>
       <c r="C59" t="n">
         <v>19.37188003693402</v>
@@ -1443,6 +1619,9 @@
       </c>
       <c r="E59" t="n">
         <v>0.4206998249752442</v>
+      </c>
+      <c r="F59" t="n">
+        <v>4.566202762782357</v>
       </c>
     </row>
     <row r="60">
@@ -1450,7 +1629,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="2" t="n">
-        <v>45283.41666666666</v>
+        <v>45285.41666666666</v>
       </c>
       <c r="C60" t="n">
         <v>18.31659102237377</v>
@@ -1460,6 +1639,9 @@
       </c>
       <c r="E60" t="n">
         <v>0.8081435704730688</v>
+      </c>
+      <c r="F60" t="n">
+        <v>2.556711994304689</v>
       </c>
     </row>
     <row r="61">
@@ -1467,7 +1649,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="2" t="n">
-        <v>45283.45833333334</v>
+        <v>45285.45833333334</v>
       </c>
       <c r="C61" t="n">
         <v>20.27731231534285</v>
@@ -1477,6 +1659,9 @@
       </c>
       <c r="E61" t="n">
         <v>4.492770942635397</v>
+      </c>
+      <c r="F61" t="n">
+        <v>2.507581473435998</v>
       </c>
     </row>
     <row r="62">
@@ -1484,7 +1669,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="2" t="n">
-        <v>45283.5</v>
+        <v>45285.5</v>
       </c>
       <c r="C62" t="n">
         <v>20.72074102782637</v>
@@ -1494,6 +1679,9 @@
       </c>
       <c r="E62" t="n">
         <v>3.03214529829795</v>
+      </c>
+      <c r="F62" t="n">
+        <v>3.991475894833876</v>
       </c>
     </row>
     <row r="63">
@@ -1501,7 +1689,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="2" t="n">
-        <v>45283.54166666666</v>
+        <v>45285.54166666666</v>
       </c>
       <c r="C63" t="n">
         <v>19.89944322241727</v>
@@ -1511,6 +1699,9 @@
       </c>
       <c r="E63" t="n">
         <v>0.04598525808314824</v>
+      </c>
+      <c r="F63" t="n">
+        <v>3.249819653888826</v>
       </c>
     </row>
     <row r="64">
@@ -1518,7 +1709,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="2" t="n">
-        <v>45283.58333333334</v>
+        <v>45285.58333333334</v>
       </c>
       <c r="C64" t="n">
         <v>23.8011625640635</v>
@@ -1528,6 +1719,9 @@
       </c>
       <c r="E64" t="n">
         <v>0.5073577143301605</v>
+      </c>
+      <c r="F64" t="n">
+        <v>3.509834386288517</v>
       </c>
     </row>
     <row r="65">
@@ -1535,7 +1729,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="2" t="n">
-        <v>45283.625</v>
+        <v>45285.625</v>
       </c>
       <c r="C65" t="n">
         <v>20.49727328685513</v>
@@ -1545,6 +1739,9 @@
       </c>
       <c r="E65" t="n">
         <v>3.317508845540279</v>
+      </c>
+      <c r="F65" t="n">
+        <v>3.978963347180505</v>
       </c>
     </row>
     <row r="66">
@@ -1552,7 +1749,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="2" t="n">
-        <v>45283.66666666666</v>
+        <v>45285.66666666666</v>
       </c>
       <c r="C66" t="n">
         <v>19.96654156781166</v>
@@ -1562,6 +1759,9 @@
       </c>
       <c r="E66" t="n">
         <v>0.02530791923109343</v>
+      </c>
+      <c r="F66" t="n">
+        <v>4.450026709087831</v>
       </c>
     </row>
     <row r="67">
@@ -1569,7 +1769,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="2" t="n">
-        <v>45283.70833333334</v>
+        <v>45285.70833333334</v>
       </c>
       <c r="C67" t="n">
         <v>21.79887258210774</v>
@@ -1579,6 +1779,9 @@
       </c>
       <c r="E67" t="n">
         <v>0.8040402570874933</v>
+      </c>
+      <c r="F67" t="n">
+        <v>1.689975784257679</v>
       </c>
     </row>
     <row r="68">
@@ -1586,7 +1789,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="2" t="n">
-        <v>45283.75</v>
+        <v>45285.75</v>
       </c>
       <c r="C68" t="n">
         <v>18.98646957482334</v>
@@ -1596,6 +1799,9 @@
       </c>
       <c r="E68" t="n">
         <v>2.743668946832931</v>
+      </c>
+      <c r="F68" t="n">
+        <v>1.87791476319972</v>
       </c>
     </row>
     <row r="69">
@@ -1603,7 +1809,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="2" t="n">
-        <v>45283.79166666666</v>
+        <v>45285.79166666666</v>
       </c>
       <c r="C69" t="n">
         <v>23.61537886527828</v>
@@ -1613,6 +1819,9 @@
       </c>
       <c r="E69" t="n">
         <v>3.459475988463466</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.469909699204345</v>
       </c>
     </row>
     <row r="70">
@@ -1620,7 +1829,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="2" t="n">
-        <v>45283.83333333334</v>
+        <v>45285.83333333334</v>
       </c>
       <c r="C70" t="n">
         <v>18.52185450575839</v>
@@ -1630,6 +1839,9 @@
       </c>
       <c r="E70" t="n">
         <v>3.259806297513003</v>
+      </c>
+      <c r="F70" t="n">
+        <v>2.89140070498087</v>
       </c>
     </row>
     <row r="71">
@@ -1637,7 +1849,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="2" t="n">
-        <v>45283.875</v>
+        <v>45285.875</v>
       </c>
       <c r="C71" t="n">
         <v>24.90820855620362</v>
@@ -1647,6 +1859,9 @@
       </c>
       <c r="E71" t="n">
         <v>1.121346547302799</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.1797113689837104</v>
       </c>
     </row>
     <row r="72">
@@ -1654,7 +1869,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="2" t="n">
-        <v>45283.91666666666</v>
+        <v>45285.91666666666</v>
       </c>
       <c r="C72" t="n">
         <v>23.4057133850766</v>
@@ -1664,6 +1879,9 @@
       </c>
       <c r="E72" t="n">
         <v>3.560896106737679</v>
+      </c>
+      <c r="F72" t="n">
+        <v>2.327990090662301</v>
       </c>
     </row>
     <row r="73">
@@ -1671,7 +1889,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="2" t="n">
-        <v>45283.95833333334</v>
+        <v>45285.95833333334</v>
       </c>
       <c r="C73" t="n">
         <v>19.39100977073921</v>
@@ -1681,6 +1899,9 @@
       </c>
       <c r="E73" t="n">
         <v>1.186245437484</v>
+      </c>
+      <c r="F73" t="n">
+        <v>2.713223173537883</v>
       </c>
     </row>
   </sheetData>

</xml_diff>